<commit_message>
std_IS completed and verified. WIP std_BS
- std_IS completed verified against filing. Code refactored.
- std_BS in progress.
- transpose_df fixed removing non numeric columns
</commit_message>
<xml_diff>
--- a/data/standardized_BS.xlsx
+++ b/data/standardized_BS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielepicheo/GitHub/R /SEC_data_analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD673ECA-E4D1-BD4C-8473-4ADAA5307C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D395AF-24C3-B84E-9091-B7F4D0C1F8C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="12340" windowHeight="20000" xr2:uid="{4802AE4D-B274-A94A-943F-E5938A0AE0CD}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="113">
   <si>
-    <t>standardized_balancesheet_label</t>
-  </si>
-  <si>
     <t>Total Accounts Receivable</t>
   </si>
   <si>
@@ -375,6 +372,9 @@
   </si>
   <si>
     <t>BS</t>
+  </si>
+  <si>
+    <t>standardized_label</t>
   </si>
 </sst>
 </file>
@@ -783,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6F0AFE-E52E-334A-8161-7EB63B8B31FB}">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E40"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -798,683 +798,683 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="D1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>65</v>
-      </c>
       <c r="D14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>103</v>
-      </c>
       <c r="D15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>21</v>
-      </c>
       <c r="C21" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="C26" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>84</v>
-      </c>
       <c r="D26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E31" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="D32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B33" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>87</v>
-      </c>
       <c r="D33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B34" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>89</v>
-      </c>
       <c r="D34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D35" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E35" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B36" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>93</v>
-      </c>
       <c r="D36" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E36" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B37" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>95</v>
-      </c>
       <c r="D37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D38" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E38" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E39" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D40" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E40" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New: calculate_trailing_month - publish quarto
- Utils.R function to calculate trailing months. Updating standardized quarterly format.
- Publication of the Quarto website
</commit_message>
<xml_diff>
--- a/data/standardized_BS.xlsx
+++ b/data/standardized_BS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielepicheo/GitHub/R /SEC_data_analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D395AF-24C3-B84E-9091-B7F4D0C1F8C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C54079-EAEB-EB4F-8A80-EEC831F28008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="860" windowWidth="12340" windowHeight="20000" xr2:uid="{4802AE4D-B274-A94A-943F-E5938A0AE0CD}"/>
+    <workbookView xWindow="25580" yWindow="1300" windowWidth="24480" windowHeight="20000" xr2:uid="{4802AE4D-B274-A94A-943F-E5938A0AE0CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="114">
   <si>
     <t>Total Accounts Receivable</t>
   </si>
@@ -375,6 +375,9 @@
   </si>
   <si>
     <t>standardized_label</t>
+  </si>
+  <si>
+    <t>Total of all stockholders' equity (deficit) items, net of receivables from officers, directors, owners, and affiliates of the entity which is directly or indirectly attributable to that ownership interest in subsidiary equity which is not attributable to the parent (that is, noncontrolling interest, previously referred to as minority interest).</t>
   </si>
 </sst>
 </file>
@@ -781,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6F0AFE-E52E-334A-8161-7EB63B8B31FB}">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1427,14 +1430,14 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>95</v>
+      <c r="A38" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>93</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>30</v>
+        <v>113</v>
       </c>
       <c r="D38" t="s">
         <v>110</v>
@@ -1447,33 +1450,50 @@
       <c r="A39" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39" t="s">
+        <v>110</v>
+      </c>
+      <c r="E39" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C40" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D39" t="s">
-        <v>110</v>
-      </c>
-      <c r="E39" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
+      <c r="D40" t="s">
+        <v>110</v>
+      </c>
+      <c r="E40" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C41" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D40" t="s">
-        <v>110</v>
-      </c>
-      <c r="E40" t="s">
+      <c r="D41" t="s">
+        <v>110</v>
+      </c>
+      <c r="E41" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>